<commit_message>
Changed the stretching to y-axis (rotated)
</commit_message>
<xml_diff>
--- a/distance_comparisons.xlsx
+++ b/distance_comparisons.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -270,7 +270,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="11">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -282,8 +282,14 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -303,18 +309,26 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -647,7 +661,7 @@
   <dimension ref="A1:O32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K6" sqref="K6"/>
+      <selection activeCell="P35" sqref="P35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -748,11 +762,11 @@
         <v>2</v>
       </c>
       <c r="L3">
-        <f>(I$3-I3)^2</f>
+        <f>((I$3-I3)^2)</f>
         <v>0</v>
       </c>
       <c r="M3">
-        <f>((J$3-J3)^2)</f>
+        <f>$C$18*((J$3-J3)^2)</f>
         <v>0</v>
       </c>
       <c r="N3">
@@ -760,7 +774,7 @@
         <v>0</v>
       </c>
       <c r="O3">
-        <f>SQRT(SUM(L3:N3))</f>
+        <f t="shared" ref="O3:O14" si="0">SQRT(SUM(L3:N3))</f>
         <v>0</v>
       </c>
     </row>
@@ -790,32 +804,32 @@
         <v>2</v>
       </c>
       <c r="I4" s="1">
-        <f t="shared" ref="I4:I8" si="0">F4*$G$18+G4*(-$F$18)</f>
+        <f t="shared" ref="I4:I8" si="1">F4*$G$18+G4*(-$F$18)</f>
         <v>0.63775642706553293</v>
       </c>
       <c r="J4" s="1">
-        <f t="shared" ref="J4:J8" si="1">F4*($F$18)+G4*$G$18</f>
+        <f t="shared" ref="J4:J8" si="2">F4*($F$18)+G4*$G$18</f>
         <v>5.3472672216503829</v>
       </c>
       <c r="K4" s="1">
-        <f t="shared" ref="K4:K14" si="2">H4</f>
+        <f t="shared" ref="K4:K14" si="3">H4</f>
         <v>2</v>
       </c>
       <c r="L4">
-        <f>$C$18*((I$3-I4)^2)</f>
-        <v>9.3301270189221945</v>
+        <f t="shared" ref="L4:L8" si="4">((I$3-I4)^2)</f>
+        <v>0.93301270189221941</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M8" si="3">((J$3-J4)^2)</f>
-        <v>6.698729810778066E-2</v>
+        <f t="shared" ref="M4:M8" si="5">$C$18*((J$3-J4)^2)</f>
+        <v>0.66987298107780657</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N8" si="4">$D$18*((K$3-K4)^2)</f>
+        <f t="shared" ref="N4:N8" si="6">$D$18*((K$3-K4)^2)</f>
         <v>0</v>
       </c>
       <c r="O4">
-        <f>SQRT(SUM(L4:N4))</f>
-        <v>3.0654713042254982</v>
+        <f t="shared" si="0"/>
+        <v>1.2660512165667019</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -844,32 +858,32 @@
         <v>2</v>
       </c>
       <c r="I5" s="1">
+        <f t="shared" si="1"/>
+        <v>1.6036822533546014</v>
+      </c>
+      <c r="J5" s="1">
+        <f t="shared" si="2"/>
+        <v>5.6060862667529037</v>
+      </c>
+      <c r="K5" s="1">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="L5">
+        <f t="shared" si="4"/>
+        <v>3.7320508075688785</v>
+      </c>
+      <c r="M5">
+        <f t="shared" si="5"/>
+        <v>2.6794919243112263</v>
+      </c>
+      <c r="N5">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="O5">
         <f t="shared" si="0"/>
-        <v>1.6036822533546014</v>
-      </c>
-      <c r="J5" s="1">
-        <f t="shared" si="1"/>
-        <v>5.6060862667529037</v>
-      </c>
-      <c r="K5" s="1">
-        <f t="shared" si="2"/>
-        <v>2</v>
-      </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L8" si="5">$C$18*((I$3-I5)^2)</f>
-        <v>37.320508075688785</v>
-      </c>
-      <c r="M5">
-        <f t="shared" si="3"/>
-        <v>0.26794919243112264</v>
-      </c>
-      <c r="N5">
-        <f t="shared" si="4"/>
-        <v>0</v>
-      </c>
-      <c r="O5">
-        <f>SQRT(SUM(L5:N5))</f>
-        <v>6.1309426084509964</v>
+        <v>2.5321024331334039</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -898,32 +912,32 @@
         <v>1</v>
       </c>
       <c r="I6" s="1">
+        <f t="shared" si="1"/>
+        <v>-6.9350354121014646E-2</v>
+      </c>
+      <c r="J6" s="1">
+        <f t="shared" si="2"/>
+        <v>4.1225223502587944</v>
+      </c>
+      <c r="K6" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L6">
+        <f t="shared" si="4"/>
+        <v>6.698729810778066E-2</v>
+      </c>
+      <c r="M6">
+        <f t="shared" si="5"/>
+        <v>9.3301270189221839</v>
+      </c>
+      <c r="N6">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="O6">
         <f t="shared" si="0"/>
-        <v>-6.9350354121014646E-2</v>
-      </c>
-      <c r="J6" s="1">
-        <f t="shared" si="1"/>
-        <v>4.1225223502587944</v>
-      </c>
-      <c r="K6" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L6">
-        <f t="shared" si="5"/>
-        <v>0.66987298107780657</v>
-      </c>
-      <c r="M6">
-        <f t="shared" si="3"/>
-        <v>0.9330127018922183</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="O6">
-        <f>SQRT(SUM(L6:N6))</f>
-        <v>4.0746638736182925</v>
+        <v>4.9393435107339894</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -952,32 +966,32 @@
         <v>1</v>
       </c>
       <c r="I7" s="1">
+        <f t="shared" si="1"/>
+        <v>0.89657547216805367</v>
+      </c>
+      <c r="J7" s="1">
+        <f t="shared" si="2"/>
+        <v>4.3813413953613143</v>
+      </c>
+      <c r="K7" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L7">
+        <f t="shared" si="4"/>
+        <v>1.4999999999999998</v>
+      </c>
+      <c r="M7">
+        <f t="shared" si="5"/>
+        <v>5.0000000000000053</v>
+      </c>
+      <c r="N7">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="O7">
         <f t="shared" si="0"/>
-        <v>0.89657547216805367</v>
-      </c>
-      <c r="J7" s="1">
-        <f t="shared" si="1"/>
-        <v>4.3813413953613143</v>
-      </c>
-      <c r="K7" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="5"/>
-        <v>14.999999999999998</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="3"/>
-        <v>0.50000000000000056</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="O7">
-        <f>SQRT(SUM(L7:N7))</f>
-        <v>5.5226805085936306</v>
+        <v>4.6368092477478529</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -1006,32 +1020,32 @@
         <v>1</v>
       </c>
       <c r="I8" s="1">
+        <f t="shared" si="1"/>
+        <v>1.8625012984571221</v>
+      </c>
+      <c r="J8" s="1">
+        <f t="shared" si="2"/>
+        <v>4.6401604404638359</v>
+      </c>
+      <c r="K8" s="1">
+        <f t="shared" si="3"/>
+        <v>1</v>
+      </c>
+      <c r="L8">
+        <f t="shared" si="4"/>
+        <v>4.7990381056766589</v>
+      </c>
+      <c r="M8">
+        <f t="shared" si="5"/>
+        <v>2.0096189432334159</v>
+      </c>
+      <c r="N8">
+        <f t="shared" si="6"/>
+        <v>15</v>
+      </c>
+      <c r="O8">
         <f t="shared" si="0"/>
-        <v>1.8625012984571221</v>
-      </c>
-      <c r="J8" s="1">
-        <f t="shared" si="1"/>
-        <v>4.6401604404638359</v>
-      </c>
-      <c r="K8" s="1">
-        <f t="shared" si="2"/>
-        <v>1</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="5"/>
-        <v>47.990381056766587</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="3"/>
-        <v>0.20096189432334161</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="4"/>
-        <v>15</v>
-      </c>
-      <c r="O8">
-        <f>SQRT(SUM(L8:N8))</f>
-        <v>7.949298267840371</v>
+        <v>4.6699739880335605</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -1068,15 +1082,15 @@
         <v>5</v>
       </c>
       <c r="K9" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L9">
-        <f>$C$19*((I$9-I9)^2)</f>
+        <f>((I$9-I9)^2)</f>
         <v>0</v>
       </c>
       <c r="M9">
-        <f>((J$9-J9)^2)</f>
+        <f>$C$19*((J$9-J9)^2)</f>
         <v>0</v>
       </c>
       <c r="N9">
@@ -1084,7 +1098,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <f>SQRT(SUM(L9:N9))</f>
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
@@ -1114,32 +1128,32 @@
         <v>2</v>
       </c>
       <c r="I10" s="1">
-        <f t="shared" ref="I10:I14" si="6">F10*$G$19+G10*(-$F$19)</f>
+        <f t="shared" ref="I10:I14" si="7">F10*$G$19+G10*(-$F$19)</f>
         <v>2</v>
       </c>
       <c r="J10" s="1">
-        <f t="shared" ref="J10:J14" si="7">F10*($F$19)+G10*$G$19</f>
+        <f t="shared" ref="J10:J14" si="8">F10*($F$19)+G10*$G$19</f>
         <v>5</v>
       </c>
       <c r="K10" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:L14" si="8">$C$19*((I$9-I10)^2)</f>
-        <v>10</v>
+        <f t="shared" ref="L10:L14" si="9">((I$9-I10)^2)</f>
+        <v>1</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10:M14" si="9">((J$9-J10)^2)</f>
+        <f t="shared" ref="M10:M14" si="10">$C$19*((J$9-J10)^2)</f>
         <v>0</v>
       </c>
       <c r="N10">
-        <f t="shared" ref="N10:N14" si="10">$D$19*((K$9-K10)^2)</f>
+        <f t="shared" ref="N10:N14" si="11">$D$19*((K$9-K10)^2)</f>
         <v>0</v>
       </c>
       <c r="O10">
-        <f>SQRT(SUM(L10:N10))</f>
-        <v>3.1622776601683795</v>
+        <f t="shared" si="0"/>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:15">
@@ -1168,32 +1182,32 @@
         <v>2</v>
       </c>
       <c r="I11" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="J11" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>5</v>
       </c>
       <c r="K11" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2</v>
       </c>
       <c r="L11">
-        <f t="shared" si="8"/>
-        <v>40</v>
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
       <c r="M11">
-        <f t="shared" si="9"/>
+        <f t="shared" si="10"/>
         <v>0</v>
       </c>
       <c r="N11">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="O11">
-        <f>SQRT(SUM(L11:N11))</f>
-        <v>6.324555320336759</v>
+        <f t="shared" si="0"/>
+        <v>2</v>
       </c>
     </row>
     <row r="12" spans="1:15">
@@ -1222,32 +1236,32 @@
         <v>1</v>
       </c>
       <c r="I12" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>1</v>
       </c>
       <c r="J12" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="K12" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L12">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="M12">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="N12">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O12">
-        <f>SQRT(SUM(L12:N12))</f>
-        <v>2.4494897427831779</v>
+        <f t="shared" si="0"/>
+        <v>3.872983346207417</v>
       </c>
     </row>
     <row r="13" spans="1:15">
@@ -1276,31 +1290,31 @@
         <v>1</v>
       </c>
       <c r="I13" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>2</v>
       </c>
       <c r="J13" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="K13" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L13">
-        <f t="shared" si="8"/>
+        <f t="shared" si="9"/>
+        <v>1</v>
+      </c>
+      <c r="M13">
+        <f t="shared" si="10"/>
         <v>10</v>
       </c>
-      <c r="M13">
-        <f t="shared" si="9"/>
-        <v>1</v>
-      </c>
       <c r="N13">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O13">
-        <f>SQRT(SUM(L13:N13))</f>
+        <f t="shared" si="0"/>
         <v>4</v>
       </c>
     </row>
@@ -1330,32 +1344,32 @@
         <v>1</v>
       </c>
       <c r="I14" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>3</v>
       </c>
       <c r="J14" s="1">
-        <f t="shared" si="7"/>
+        <f t="shared" si="8"/>
         <v>4</v>
       </c>
       <c r="K14" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="L14">
-        <f t="shared" si="8"/>
-        <v>40</v>
+        <f t="shared" si="9"/>
+        <v>4</v>
       </c>
       <c r="M14">
-        <f t="shared" si="9"/>
-        <v>1</v>
+        <f t="shared" si="10"/>
+        <v>10</v>
       </c>
       <c r="N14">
-        <f t="shared" si="10"/>
+        <f t="shared" si="11"/>
         <v>5</v>
       </c>
       <c r="O14">
-        <f>SQRT(SUM(L14:N14))</f>
-        <v>6.7823299831252681</v>
+        <f t="shared" si="0"/>
+        <v>4.358898943540674</v>
       </c>
     </row>
     <row r="16" spans="1:15">
@@ -1463,20 +1477,20 @@
       <c r="B23" s="6">
         <v>0</v>
       </c>
-      <c r="C23" s="10">
-        <v>3.0649999999999999</v>
-      </c>
-      <c r="D23" s="10">
-        <v>6.1310000000000002</v>
-      </c>
-      <c r="E23" s="10">
-        <v>4.0750000000000002</v>
-      </c>
-      <c r="F23" s="10">
-        <v>5.5229999999999997</v>
-      </c>
-      <c r="G23" s="11">
-        <v>7.9489999999999998</v>
+      <c r="C23" s="6">
+        <v>1.266</v>
+      </c>
+      <c r="D23" s="6">
+        <v>2.532</v>
+      </c>
+      <c r="E23" s="6">
+        <v>4.9390000000000001</v>
+      </c>
+      <c r="F23" s="6">
+        <v>4.6369999999999996</v>
+      </c>
+      <c r="G23" s="19">
+        <v>4.67</v>
       </c>
     </row>
     <row r="24" spans="1:7">
@@ -1499,20 +1513,20 @@
       <c r="B25" s="9">
         <v>0</v>
       </c>
-      <c r="C25" s="12">
-        <v>3.1619999999999999</v>
-      </c>
-      <c r="D25" s="12">
-        <v>6.3250000000000002</v>
-      </c>
-      <c r="E25" s="12">
-        <v>2.4489999999999998</v>
-      </c>
-      <c r="F25" s="12">
+      <c r="C25" s="9">
+        <v>1</v>
+      </c>
+      <c r="D25" s="9">
+        <v>2</v>
+      </c>
+      <c r="E25" s="9">
+        <v>3.8730000000000002</v>
+      </c>
+      <c r="F25" s="9">
         <v>4</v>
       </c>
-      <c r="G25" s="13">
-        <v>6.782</v>
+      <c r="G25" s="20">
+        <v>4.359</v>
       </c>
     </row>
     <row r="26" spans="1:7">
@@ -1555,23 +1569,23 @@
       </c>
       <c r="C29" s="10">
         <f>O4</f>
-        <v>3.0654713042254982</v>
+        <v>1.2660512165667019</v>
       </c>
       <c r="D29" s="10">
         <f>O5</f>
-        <v>6.1309426084509964</v>
+        <v>2.5321024331334039</v>
       </c>
       <c r="E29" s="10">
         <f>O6</f>
-        <v>4.0746638736182925</v>
+        <v>4.9393435107339894</v>
       </c>
       <c r="F29" s="10">
         <f>O7</f>
-        <v>5.5226805085936306</v>
+        <v>4.6368092477478529</v>
       </c>
       <c r="G29" s="11">
         <f>O8</f>
-        <v>7.949298267840371</v>
+        <v>4.6699739880335605</v>
       </c>
     </row>
     <row r="30" spans="1:7">
@@ -1597,15 +1611,15 @@
       </c>
       <c r="C31" s="12">
         <f>O10</f>
-        <v>3.1622776601683795</v>
+        <v>1</v>
       </c>
       <c r="D31" s="12">
         <f>O11</f>
-        <v>6.324555320336759</v>
+        <v>2</v>
       </c>
       <c r="E31" s="12">
         <f>O12</f>
-        <v>2.4494897427831779</v>
+        <v>3.872983346207417</v>
       </c>
       <c r="F31" s="12">
         <f>O13</f>
@@ -1613,7 +1627,7 @@
       </c>
       <c r="G31" s="13">
         <f>O14</f>
-        <v>6.7823299831252681</v>
+        <v>4.358898943540674</v>
       </c>
     </row>
     <row r="32" spans="1:7">

</xml_diff>